<commit_message>
added additional page content to translate doc
</commit_message>
<xml_diff>
--- a/SurgeonPortal.Api/ClientApp/language-test/translations.xlsx
+++ b/SurgeonPortal.Api/ClientApp/language-test/translations.xlsx
@@ -6,7 +6,7 @@
     <sheet name="Translation Keys for Export" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Translation Keys for Export'!$A$1:$C$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Translation Keys for Export'!$A$1:$D$128</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -409,6 +409,7 @@
     <col min="2" max="2" customWidth="1" width="30"/>
     <col min="3" max="3" customWidth="1" width="30"/>
     <col min="4" max="4" customWidth="1" width="30"/>
+    <col min="5" max="5" customWidth="1" width="30"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -421,780 +422,1050 @@
       <c r="C1" t="str">
         <v>comments</v>
       </c>
+      <c r="D1" t="str">
+        <v>notes</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>DASHBOARD.ACTION_CARDS.APPLY_BTN</v>
+        <v>CME.TITLE</v>
       </c>
       <c r="B2" t="str">
-        <v>Apply for Exam</v>
-      </c>
-      <c r="C2" t="str">
-        <v>This is a really cool button that we love</v>
+        <v>CME Repository</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>DASHBOARD.ACTION_CARDS.APPLY_SUBTITLE</v>
+        <v>CME.SUBTITLE</v>
       </c>
       <c r="B3" t="str">
-        <v>QE applications are not yet available. Check back on {{date}}</v>
+        <v>CME requirements for the Continuous Certification (CC) Program are &lt;strong&gt;150 category 1 CME credits&lt;/strong&gt; earned over the last five calendar years, &lt;strong&gt;50 of which must be self-assesment credits.&lt;/strong&gt;</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>DASHBOARD.ACTION_CARDS.APPLY_TITLE</v>
+        <v>CME.TOOLTIP</v>
       </c>
       <c r="B4" t="str">
-        <v>Apply for a Qualified Exam</v>
+        <v>Stay on track with CME requirements by averaging 30 credits per year.</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>DASHBOARD.ACTION_CARDS.CCR_BTN</v>
+        <v>CME.HELPTEXT</v>
       </c>
       <c r="B5" t="str">
-        <v>See Requirements</v>
+        <v>Credits and ABS Waivers dropping off are those that were earned more than five years ago from today. You may see an increase in the number of credits needed the next time you login if you have CME that is expiring between now and the end of the year. Refer to the itemized CME section for specific CME activities that may drop off soon.</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>DASHBOARD.ACTION_CARDS.CCR_SUBTITLE</v>
+        <v>CME.ITEMIZED_CME.TITLE</v>
       </c>
       <c r="B6" t="str">
-        <v>Click here to view your current Continuous Certification progress and complete any remaining requirements.</v>
+        <v>Itemized CME</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>DASHBOARD.ACTION_CARDS.CCR_TITLE</v>
+        <v>CME.WAIVERS.TITLE</v>
       </c>
       <c r="B7" t="str">
-        <v>Continuous Certification Requirements</v>
-      </c>
-      <c r="C7" t="str">
-        <v>THis is the coolest tag that we have ever written. As a matter of fact we would love to write 50 more, just like this.</v>
+        <v>Itemized ABS Waivers that Reduce Your CME Requirements</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>DASHBOARD.ACTION_CARDS.CME_BTN</v>
+        <v>CME.WAIVERS.SUBTITLE</v>
       </c>
       <c r="B8" t="str">
-        <v>View Your CME</v>
+        <v>Listed below are activities you completed (e.g., a CCA module) during the current five-year period that have reduced your overall CME requirements.</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>DASHBOARD.ACTION_CARDS.CME_SUBTITLE</v>
+        <v>DASHBOARD.ACTION_CARDS.APPLY_BTN</v>
       </c>
       <c r="B9" t="str">
-        <v>Click here to view your current CME Credits and keep track of your requirements for the Continuous Certification Program.</v>
+        <v>Apply for Exam</v>
+      </c>
+      <c r="C9" t="str">
+        <v>This is a really cool button that we love</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>DASHBOARD.ACTION_CARDS.CME_TITLE</v>
+        <v>DASHBOARD.ACTION_CARDS.APPLY_SUBTITLE</v>
       </c>
       <c r="B10" t="str">
-        <v>Continuing Medical Education (CME)</v>
+        <v>QE applications are not yet available. Check back on {{date}}</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>DASHBOARD.ACTION_CARDS.GME_BTN</v>
+        <v>DASHBOARD.ACTION_CARDS.APPLY_TITLE</v>
       </c>
       <c r="B11" t="str">
-        <v>View Your GME</v>
+        <v>Apply for a Qualified Exam</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>DASHBOARD.ACTION_CARDS.GME_SUBTITLE</v>
+        <v>DASHBOARD.ACTION_CARDS.CCR_BTN</v>
       </c>
       <c r="B12" t="str">
-        <v>Click here to view your current GME progress and to add rotations to your GME history.</v>
+        <v>See Requirements</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>DASHBOARD.ACTION_CARDS.GME_TITLE</v>
+        <v>DASHBOARD.ACTION_CARDS.CCR_SUBTITLE</v>
       </c>
       <c r="B13" t="str">
-        <v>Graduate Medical Education (GME)</v>
+        <v>Click here to view your current Continuous Certification progress and complete any remaining requirements.</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>DASHBOARD.ACTION_CARDS.REGISTER_BTN</v>
+        <v>DASHBOARD.ACTION_CARDS.CCR_TITLE</v>
       </c>
       <c r="B14" t="str">
-        <v>Apply Now</v>
+        <v>Continuous Certification Requirements</v>
+      </c>
+      <c r="C14" t="str">
+        <v>THis is the coolest tag that we have ever written. As a matter of fact we would love to write 50 more, just like this.</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>DASHBOARD.ACTION_CARDS.REGISTER_SUBTITLE</v>
+        <v>DASHBOARD.ACTION_CARDS.CME_BTN</v>
       </c>
       <c r="B15" t="str">
-        <v>Click here to view and apply or register for any eligible exams.</v>
+        <v>View Your CME</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>DASHBOARD.ACTION_CARDS.REGISTER_TITLE</v>
+        <v>DASHBOARD.ACTION_CARDS.CME_SUBTITLE</v>
       </c>
       <c r="B16" t="str">
-        <v>Apply and Register</v>
+        <v>Click here to view your current CME Credits and keep track of your requirements for the Continuous Certification Program.</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>DASHBOARD.HIGHLIGHT_CARDS.DOCUMENTS_BTN</v>
+        <v>DASHBOARD.ACTION_CARDS.CME_TITLE</v>
       </c>
       <c r="B17" t="str">
-        <v>View Your Documents</v>
+        <v>Continuing Medical Education (CME)</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>DASHBOARD.HIGHLIGHT_CARDS.DOCUMENTS_SUBTITLE</v>
+        <v>DASHBOARD.ACTION_CARDS.GME_BTN</v>
       </c>
       <c r="B18" t="str">
-        <v>Click here to view all of your current document and certificate uploads.</v>
+        <v>View Your GME</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>DASHBOARD.HIGHLIGHT_CARDS.DOCUMENTS_TITLE</v>
+        <v>DASHBOARD.ACTION_CARDS.GME_SUBTITLE</v>
       </c>
       <c r="B19" t="str">
-        <v>Documents</v>
+        <v>Click here to view your current GME progress and to add rotations to your GME history.</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>DASHBOARD.HIGHLIGHT_CARDS.EXAMREGISTRATION_TITLE</v>
+        <v>DASHBOARD.ACTION_CARDS.GME_TITLE</v>
       </c>
       <c r="B20" t="str">
-        <v>Upcoming Exam Registration</v>
+        <v>Graduate Medical Education (GME)</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>DASHBOARD.HIGHLIGHT_CARDS.UPCOMINGEXAMS_SUBTITLE</v>
+        <v>DASHBOARD.ACTION_CARDS.REGISTER_BTN</v>
       </c>
       <c r="B21" t="str">
-        <v>You will be able to find more information about upcoming exams here as that information becomes available.</v>
+        <v>Apply Now</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>DASHBOARD.HIGHLIGHT_CARDS.UPCOMINGEXAMS_TITLE</v>
+        <v>DASHBOARD.ACTION_CARDS.REGISTER_SUBTITLE</v>
       </c>
       <c r="B22" t="str">
-        <v>Next General Surgery QE -  {{date}}</v>
+        <v>Click here to view and apply or register for any eligible exams.</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>DASHBOARD.LASTLOGIN</v>
+        <v>DASHBOARD.ACTION_CARDS.REGISTER_TITLE</v>
       </c>
       <c r="B23" t="str">
-        <v>&lt;strong&gt;Last Login:&lt;/strong&gt; {{lastLogin}}</v>
+        <v>Apply and Register</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>DASHBOARD.STATUS</v>
+        <v>DASHBOARD.HIGHLIGHT_CARDS.DOCUMENTS_BTN</v>
       </c>
       <c r="B24" t="str">
-        <v>&lt;strong&gt;Current Status:&lt;/strong&gt; {{status}}</v>
+        <v>View Your Documents</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>DASHBOARD.SUBTITLE</v>
+        <v>DASHBOARD.HIGHLIGHT_CARDS.DOCUMENTS_SUBTITLE</v>
       </c>
       <c r="B25" t="str">
-        <v>Hello, {{user}}!</v>
+        <v>Click here to view all of your current document and certificate uploads.</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>DASHBOARD.TITLE</v>
+        <v>DASHBOARD.HIGHLIGHT_CARDS.DOCUMENTS_TITLE</v>
       </c>
       <c r="B26" t="str">
-        <v>Dashboard</v>
+        <v>Documents</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>EXAMSCORING.DASHBOARD.AGENDA_BTN</v>
+        <v>DASHBOARD.HIGHLIGHT_CARDS.EXAMREGISTRATION_TITLE</v>
       </c>
       <c r="B27" t="str">
-        <v>Download Agenda</v>
+        <v>Upcoming Exam Registration</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>EXAMSCORING.DASHBOARD.AGENDA_SUBTITLE</v>
+        <v>DASHBOARD.HIGHLIGHT_CARDS.UPCOMINGEXAMS_SUBTITLE</v>
       </c>
       <c r="B28" t="str">
-        <v>Your agenda can be found here once it has been finalized.</v>
+        <v>You will be able to find more information about upcoming exams here as that information becomes available.</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>EXAMSCORING.DASHBOARD.AGENDA_TITLE</v>
+        <v>DASHBOARD.HIGHLIGHT_CARDS.UPCOMINGEXAMS_TITLE</v>
       </c>
       <c r="B29" t="str">
-        <v>Your Examination Agenda</v>
+        <v>Next General Surgery QE -  {{date}}</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>EXAMSCORING.DASHBOARD.CERTIFYING_NORESULTS</v>
+        <v>DASHBOARD.LASTLOGIN</v>
       </c>
       <c r="B30" t="str">
-        <v>Links to certifying examinations and examinee scoring pages can be found here on the day of the exam.</v>
+        <v>&lt;strong&gt;Last Login:&lt;/strong&gt; {{lastLogin}}</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>EXAMSCORING.DASHBOARD.CERTIFYING_TITLE</v>
+        <v>DASHBOARD.STATUS</v>
       </c>
       <c r="B31" t="str">
-        <v>Certifying Examinations for {{date}}</v>
+        <v>&lt;strong&gt;Current Status:&lt;/strong&gt; {{status}}</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>EXAMSCORING.DASHBOARD.CONFLICTS_BTN</v>
+        <v>DASHBOARD.SUBTITLE</v>
       </c>
       <c r="B32" t="str">
-        <v>Download Conflicts</v>
+        <v>Hello, {{user}}!</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>EXAMSCORING.DASHBOARD.CONFLICTS_SUBTITLE</v>
+        <v>DASHBOARD.TITLE</v>
       </c>
       <c r="B33" t="str">
-        <v>Your conflicts report can be found here once is has been finalized.</v>
+        <v>Dashboard</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>EXAMSCORING.DASHBOARD.CONFLICTS_TITLE</v>
+        <v>DOCUMENTS.TITLE</v>
       </c>
       <c r="B34" t="str">
-        <v>Your Conflicts</v>
+        <v>Documents</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>EXAMSCORING.DASHBOARD.DELIVER_BTN</v>
+        <v>DOCUMENTS.SUBTITLE</v>
       </c>
       <c r="B35" t="str">
-        <v>Begin Certifying Examinations</v>
+        <v>View all of your uploaded documents and certifications.</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>EXAMSCORING.DASHBOARD.DELIVER_SUBTITLE</v>
+        <v>EXAMSCORING.DASHBOARD.AGENDA_BTN</v>
       </c>
       <c r="B36" t="str">
-        <v>Certifying examinations along with scoring capability can be found here on exam day.</v>
+        <v>Download Agenda</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>EXAMSCORING.DASHBOARD.DELIVER_TITLE</v>
+        <v>EXAMSCORING.DASHBOARD.AGENDA_SUBTITLE</v>
       </c>
       <c r="B37" t="str">
-        <v>Deliver Certifying Examinations</v>
+        <v>Your agenda can be found here once it has been finalized.</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>EXAMSCORING.DASHBOARD.ROSTER_BTN</v>
+        <v>EXAMSCORING.DASHBOARD.AGENDA_TITLE</v>
       </c>
       <c r="B38" t="str">
-        <v>Review Exam Case Rosters</v>
+        <v>Your Examination Agenda</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>EXAMSCORING.DASHBOARD.ROSTER_SUBTITLE</v>
+        <v>EXAMSCORING.DASHBOARD.CERTIFYING_NORESULTS</v>
       </c>
       <c r="B39" t="str">
-        <v>Review the cases for the next certifying examination and add personal notes as needed. Your personal notes will display each time you present the case.</v>
+        <v>Links to certifying examinations and examinee scoring pages can be found here on the day of the exam.</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>EXAMSCORING.DASHBOARD.ROSTER_TITLE</v>
+        <v>EXAMSCORING.DASHBOARD.CERTIFYING_TITLE</v>
       </c>
       <c r="B40" t="str">
-        <v>Examination Case Rosters</v>
+        <v>Certifying Examinations for {{date}}</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>EXAMSCORING.DASHBOARD.SCORE_BTN</v>
+        <v>EXAMSCORING.DASHBOARD.CONFLICTS_BTN</v>
       </c>
       <c r="B41" t="str">
-        <v>Review Exam Scores</v>
+        <v>Download Conflicts</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>EXAMSCORING.DASHBOARD.SCORE_SUBTITLE</v>
+        <v>EXAMSCORING.DASHBOARD.CONFLICTS_SUBTITLE</v>
       </c>
       <c r="B42" t="str">
-        <v>Check the status of submitted scores and edit any that remain incomplete as soon as possible.</v>
+        <v>Your conflicts report can be found here once is has been finalized.</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>EXAMSCORING.DASHBOARD.SCORE_TITLE</v>
+        <v>EXAMSCORING.DASHBOARD.CONFLICTS_TITLE</v>
       </c>
       <c r="B43" t="str">
-        <v>Examination Scores</v>
+        <v>Your Conflicts</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>EXAMSCORING.DASHBOARD.SUBTITLE</v>
+        <v>EXAMSCORING.DASHBOARD.DELIVER_BTN</v>
       </c>
       <c r="B44" t="str">
-        <v>Welcome to your examiner's dashboard. Information on the dashboard will change based on proximity to the exam adminstration. You will be able to review cases, score examinations, and access other documentation as applicable during the exam administration process.</v>
+        <v>Begin Certifying Examinations</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>EXAMSCORING.DEFAULT_EXAM</v>
+        <v>EXAMSCORING.DASHBOARD.DELIVER_SUBTITLE</v>
       </c>
       <c r="B45" t="str">
-        <v>Certifying Examination</v>
+        <v>Certifying examinations along with scoring capability can be found here on exam day.</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>EXAMSCORING.EXAMINATION.CANDIDATE</v>
+        <v>EXAMSCORING.DASHBOARD.DELIVER_TITLE</v>
       </c>
       <c r="B46" t="str">
-        <v>&lt;strong&gt;Candidate Name:&lt;/strong&gt; {{name}}</v>
+        <v>Deliver Certifying Examinations</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>EXAMSCORING.EXAMINATION.INSTRUCTIONS</v>
+        <v>EXAMSCORING.DASHBOARD.ROSTER_BTN</v>
       </c>
       <c r="B47" t="str">
-        <v>Please read carefully the instructions below.</v>
+        <v>Review Exam Case Rosters</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>EXAMSCORING.EXAMINATION.LIST_DATE</v>
+        <v>EXAMSCORING.DASHBOARD.ROSTER_SUBTITLE</v>
       </c>
       <c r="B48" t="str">
-        <v>&lt;strong&gt;Date:&lt;/strong&gt; {{date}}</v>
+        <v>Review the cases for the next certifying examination and add personal notes as needed. Your personal notes will display each time you present the case.</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>EXAMSCORING.EXAMINATION.LIST_TITLE</v>
+        <v>EXAMSCORING.DASHBOARD.ROSTER_TITLE</v>
       </c>
       <c r="B49" t="str">
-        <v>Examinations</v>
+        <v>Examination Case Rosters</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>EXAMSCORING.EXAMINATION.SUBTITLE</v>
+        <v>EXAMSCORING.DASHBOARD.SCORE_BTN</v>
       </c>
       <c r="B50" t="str">
-        <v>Begin the oral examination process by first selecting the desired exam day from the first dropdown. You can then select the specific candidate times lot from the next dropdown. Finally, confirm your examiner user ID and you may begin the exam process.</v>
+        <v>Review Exam Scores</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>EXAMSCORING.EXAMINATION.TIME</v>
+        <v>EXAMSCORING.DASHBOARD.SCORE_SUBTITLE</v>
       </c>
       <c r="B51" t="str">
-        <v>&lt;strong&gt;Day/Time:&lt;/strong&gt; {{time}}</v>
+        <v>Check the status of submitted scores and edit any that remain incomplete as soon as possible.</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>EXAMSCORING.EXAMINATION.TITLE</v>
+        <v>EXAMSCORING.DASHBOARD.SCORE_TITLE</v>
       </c>
       <c r="B52" t="str">
-        <v>Examination</v>
+        <v>Examination Scores</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>EXAMSCORING.EXAMROSTERS.TITLE</v>
+        <v>EXAMSCORING.DASHBOARD.SUBTITLE</v>
       </c>
       <c r="B53" t="str">
-        <v>Examination Rosters</v>
+        <v>Welcome to your examiner's dashboard. Information on the dashboard will change based on proximity to the exam adminstration. You will be able to review cases, score examinations, and access other documentation as applicable during the exam administration process.</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>EXAMSCORING.EXAMSCORES.SUBTITLE</v>
+        <v>EXAMSCORING.DEFAULT_EXAM</v>
       </c>
       <c r="B54" t="str">
-        <v>Review and submit exam scores here. We kindly request that all exams are scored by the end of the exam day, at which point they will be locked down. If you need to complete or edit scores after the current exam day, please contact the psychometricians.</v>
+        <v>Certifying Examination</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>EXAMSCORING.EXAMSCORES.TITLE</v>
+        <v>EXAMSCORING.EXAMINATION.CANDIDATE</v>
       </c>
       <c r="B55" t="str">
-        <v>Examination Scores</v>
+        <v>&lt;strong&gt;Candidate Name:&lt;/strong&gt; {{name}}</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>LOGIN.PASSWORD</v>
+        <v>EXAMSCORING.EXAMINATION.INSTRUCTIONS</v>
       </c>
       <c r="B56" t="str">
-        <v>Password</v>
+        <v>Please read carefully the instructions below.</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>LOGIN.PASSWORD_ERROR</v>
+        <v>EXAMSCORING.EXAMINATION.LIST_DATE</v>
       </c>
       <c r="B57" t="str">
-        <v>The Password field is required.</v>
+        <v>&lt;strong&gt;Date:&lt;/strong&gt; {{date}}</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>LOGIN.SUBMIT_BTN</v>
+        <v>EXAMSCORING.EXAMINATION.LIST_TITLE</v>
       </c>
       <c r="B58" t="str">
-        <v>Login</v>
+        <v>Examinations</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>LOGIN.SUBTITLE</v>
+        <v>EXAMSCORING.EXAMINATION.SUBTITLE</v>
       </c>
       <c r="B59" t="str">
-        <v>Please enter your username and password to login.</v>
+        <v>Begin the oral examination process by first selecting the desired exam day from the first dropdown. You can then select the specific candidate times lot from the next dropdown. Finally, confirm your examiner user ID and you may begin the exam process.</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>LOGIN.TITLE</v>
+        <v>EXAMSCORING.EXAMINATION.TIME</v>
       </c>
       <c r="B60" t="str">
-        <v>Welcome to The American Board of Surgery Surgeon's Portal</v>
+        <v>&lt;strong&gt;Day/Time:&lt;/strong&gt; {{time}}</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>LOGIN.USERNAME</v>
+        <v>EXAMSCORING.EXAMINATION.TITLE</v>
       </c>
       <c r="B61" t="str">
-        <v>Username</v>
+        <v>Examination</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>LOGIN.USERNAME_ERROR</v>
+        <v>EXAMSCORING.EXAMROSTERS.TITLE</v>
       </c>
       <c r="B62" t="str">
-        <v>The Username field is required.</v>
+        <v>Examination Rosters</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>meta.locale</v>
+        <v>EXAMSCORING.EXAMSCORES.SUBTITLE</v>
       </c>
       <c r="B63" t="str">
-        <v>en-US</v>
-      </c>
-      <c r="C63" t="str">
-        <v>comments</v>
+        <v>Review and submit exam scores here. We kindly request that all exams are scored by the end of the exam day, at which point they will be locked down. If you need to complete or edit scores after the current exam day, please contact the psychometricians.</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>MYACCOUNT.SUBTITLE</v>
+        <v>EXAMSCORING.EXAMSCORES.TITLE</v>
       </c>
       <c r="B64" t="str">
-        <v>Enter and review your Email Address and Password here to ensure that they are accurate and up to date.</v>
+        <v>Examination Scores</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>MYACCOUNT.TITLE</v>
+        <v>GME.TITLE</v>
       </c>
       <c r="B65" t="str">
-        <v>My Account</v>
+        <v>Graduate Medical Education (GME)</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>PROFILE.SUBTITLE</v>
+        <v>GME.ROTATIONS.TITLE</v>
       </c>
       <c r="B66" t="str">
-        <v>Enter and review your Personal Information, Contact Information, Citizenship Information, and Demographic information here to ensure that it is accurate and up to date.</v>
+        <v>My GME Rotations</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>PROFILE.TITLE</v>
+        <v>GME.ROTATIONS.SUBTITLE</v>
       </c>
       <c r="B67" t="str">
-        <v>Personal Profile</v>
+        <v>Date Range Covered: {{ fromDate }} through {{ toDate }}</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>SHELL.ADD_BTN</v>
+        <v>GME.SUMMARY.TITLE</v>
       </c>
       <c r="B68" t="str">
-        <v>Add</v>
+        <v>GME Summary</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>SHELL.CANCEL_BTN</v>
+        <v>GME.SUMMARY.SUBTITLE</v>
       </c>
       <c r="B69" t="str">
-        <v>Cancel</v>
+        <v>The table below is a summary, by residency level, of your clinical experience based on the dates you entered in the table above. Columns 2 through 4 summarize the number of weeks of clinical experience during each year of residency. Column 5 is a total of weeks per residency year, of rotations devoted to the content areas of surgery. Column 6 summarizes chief resident year rotations also devoted to the content areas of surgery.</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>SHELL.CLOSE_BTN</v>
+        <v>GME.ITEMIZED_GME.TITLE</v>
       </c>
       <c r="B70" t="str">
-        <v>Close</v>
+        <v>Itemized GME</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>SHELL.CONTINUE_BTN</v>
+        <v>GME.ITEMIZED_GME.SUBTITLE</v>
       </c>
       <c r="B71" t="str">
-        <v>Continue</v>
+        <v>Document all GME rotations completely, without any gaps throughout your training years. Your program director must attest to the accuracy of your rotations, and you will be able to request an attestation from your PD upon completion of this section.</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>SHELL.COPYRIGHT</v>
+        <v>LOGIN.PASSWORD</v>
       </c>
       <c r="B72" t="str">
-        <v>@{{year}} All Rights Reserved. The American Board of Surgery</v>
+        <v>Password</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>SHELL.DELETE_BTN</v>
+        <v>LOGIN.PASSWORD_ERROR</v>
       </c>
       <c r="B73" t="str">
-        <v>Delete</v>
+        <v>The Password field is required.</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>SHELL.EDIT_BTN</v>
+        <v>LOGIN.SUBMIT_BTN</v>
       </c>
       <c r="B74" t="str">
-        <v>Edit</v>
+        <v>Login</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>SHELL.NO_BTN</v>
+        <v>LOGIN.SUBTITLE</v>
       </c>
       <c r="B75" t="str">
-        <v>No</v>
+        <v>Please enter your username and password to login.</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>SHELL.SAVE_BTN</v>
+        <v>LOGIN.TITLE</v>
       </c>
       <c r="B76" t="str">
-        <v>Save</v>
+        <v>Welcome to The American Board of Surgery Surgeon's Portal</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>SHELL.SUBMIT_BTN</v>
+        <v>LOGIN.USERNAME</v>
       </c>
       <c r="B77" t="str">
-        <v>Submit</v>
+        <v>Username</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>SHELL.YES_BTN</v>
+        <v>LOGIN.USERNAME_ERROR</v>
       </c>
       <c r="B78" t="str">
-        <v>Yes</v>
+        <v>The Username field is required.</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>SIDENAV.DASHBOARD</v>
+        <v>meta.locale</v>
       </c>
       <c r="B79" t="str">
-        <v>Dashboard</v>
+        <v>en-US</v>
+      </c>
+      <c r="C79" t="str">
+        <v>comments</v>
+      </c>
+      <c r="D79" t="str">
+        <v>notes</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>SIDENAV.PROFILE</v>
+        <v>MEDICAL_TRAINING.TITLE</v>
       </c>
       <c r="B80" t="str">
-        <v>Personal Profile</v>
+        <v>Medical Training</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>SIDENAV.MYACCOUNT</v>
+        <v>MEDICAL_TRAINING.MEDICAL_SCHOOL.TITLE</v>
       </c>
       <c r="B81" t="str">
-        <v>My Account</v>
+        <v>Medical School</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>SIDENAV.MEDICAL_TRAINING</v>
+        <v>MEDICAL_TRAINING.MEDICAL_SCHOOL.SUBTITLE</v>
       </c>
       <c r="B82" t="str">
-        <v>Medical Training</v>
+        <v>Enter and review your medical school informatuon here to ensure that it is accurate and up to date.</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>SIDENAV.PROFESSIONAL_STANDING</v>
+        <v>MEDICAL_TRAINING.RESIDENCY.TITLE</v>
       </c>
       <c r="B83" t="str">
-        <v>Professional Standing</v>
+        <v>Residency</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>SIDENAV.CME</v>
+        <v>MEDICAL_TRAINING.RESIDENCY.SUBTITLE</v>
       </c>
       <c r="B84" t="str">
-        <v>CME Repository</v>
+        <v>Enter and review your residency information here to ensure that it is accurate and up to date.</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>SIDENAV.GME</v>
+        <v>MEDICAL_TRAINING.FELLOWSHIP.TITLE</v>
       </c>
       <c r="B85" t="str">
-        <v>GME</v>
+        <v>Fellowship</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>SIDENAV.APPLY_REGISTER.MAIN</v>
+        <v>MEDICAL_TRAINING.FELLOWSHIP.SUBTITLE</v>
       </c>
       <c r="B86" t="str">
-        <v>Apply and Register</v>
+        <v>Enter and review your fellowship information here to ensure that it is accurate and up to date.</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>SIDENAV.APPLY_REGISTER.REQUIREMENTS</v>
+        <v>MEDICAL_TRAINING.CERTIFICATES.TITLE</v>
       </c>
       <c r="B87" t="str">
-        <v>Registration Requirements</v>
+        <v>Certificates</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>SIDENAV.APPLY_REGISTER.REGISTRATION</v>
+        <v>MEDICAL_TRAINING.CERTIFICATES.OTHER_CERTS_TITLE</v>
       </c>
       <c r="B88" t="str">
-        <v>Exam Registration</v>
+        <v>RPVI Certificate</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>SIDENAV.EXAM_HISTORY</v>
+        <v>MEDICAL_TRAINING.ADVANCED_TRAINING.TITLE</v>
       </c>
       <c r="B89" t="str">
-        <v>Exam History</v>
+        <v>Additional / Advanced Medical Training</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>SIDENAV.CONTINUOUS_CERTIFICATION</v>
+        <v>MYACCOUNT.SUBTITLE</v>
       </c>
       <c r="B90" t="str">
-        <v>Continuous Certification</v>
+        <v>Enter and review your Email Address and Password here to ensure that they are accurate and up to date.</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>SIDENAV.PAYMENT_HISTORY</v>
+        <v>MYACCOUNT.TITLE</v>
       </c>
       <c r="B91" t="str">
-        <v>Payment History</v>
+        <v>My Account</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>SIDENAV.DOCUMENTS</v>
+        <v>PROFESSIONAL_STANDING.TITLE</v>
       </c>
       <c r="B92" t="str">
-        <v>Documents</v>
+        <v>Professional Standing</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>SIDENAV.EXAM_SCORING.MAIN</v>
+        <v>PROFESSIONAL_STANDING.MEDICAL_LICENSE.TITLE</v>
       </c>
       <c r="B93" t="str">
-        <v>CE Examiner Home</v>
+        <v>State Medical License</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>SIDENAV.EXAM_SCORING.CASE_ROSTER</v>
+        <v>PROFESSIONAL_STANDING.MEDICAL_LICENSE.SUBTITLE</v>
       </c>
       <c r="B94" t="str">
-        <v>Examination Case Rosters</v>
+        <v>Enter and review your State Medical License information here to ensure that it is accurate and up to date.</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>SIDENAV.EXAM_SCORING.EXAMINATION</v>
+        <v>PROFESSIONAL_STANDING.APPOINTMENTS.TITLE</v>
       </c>
       <c r="B95" t="str">
-        <v>Deliver CE Exams</v>
+        <v>Current Hospital Appointments / Privileges</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
+        <v>PROFESSIONAL_STANDING.APPOINTMENTS.SUBTITLE</v>
+      </c>
+      <c r="B96" t="str">
+        <v>If you are clinically active please provide your current practice and organization type. If you are not currently clinically active please explain why as well as providing information about any current non-clinical activities.</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>PROFESSIONAL_STANDING.APPOINTMENTS.ALL_APPOINTMENTS_TITLE</v>
+      </c>
+      <c r="B97" t="str">
+        <v>All Hospital Appointments / Privileges</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>PROFESSIONAL_STANDING.SANCTIONS.TITLE</v>
+      </c>
+      <c r="B98" t="str">
+        <v>Sanctions and Ethics</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>PROFILE.SUBTITLE</v>
+      </c>
+      <c r="B99" t="str">
+        <v>Enter and review your Personal Information, Contact Information, Citizenship Information, and Demographic information here to ensure that it is accurate and up to date.</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>PROFILE.TITLE</v>
+      </c>
+      <c r="B100" t="str">
+        <v>Personal Profile</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>SHELL.ADD_BTN</v>
+      </c>
+      <c r="B101" t="str">
+        <v>Add</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>SHELL.CANCEL_BTN</v>
+      </c>
+      <c r="B102" t="str">
+        <v>Cancel</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>SHELL.CLOSE_BTN</v>
+      </c>
+      <c r="B103" t="str">
+        <v>Close</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>SHELL.CONTINUE_BTN</v>
+      </c>
+      <c r="B104" t="str">
+        <v>Continue</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>SHELL.COPYRIGHT</v>
+      </c>
+      <c r="B105" t="str">
+        <v>@{{year}} All Rights Reserved. The American Board of Surgery</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>SHELL.DELETE_BTN</v>
+      </c>
+      <c r="B106" t="str">
+        <v>Delete</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>SHELL.EDIT_BTN</v>
+      </c>
+      <c r="B107" t="str">
+        <v>Edit</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>SHELL.NO_BTN</v>
+      </c>
+      <c r="B108" t="str">
+        <v>No</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>SHELL.SAVE_BTN</v>
+      </c>
+      <c r="B109" t="str">
+        <v>Save</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>SHELL.SUBMIT_BTN</v>
+      </c>
+      <c r="B110" t="str">
+        <v>Submit</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>SHELL.YES_BTN</v>
+      </c>
+      <c r="B111" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>SIDENAV.APPLY_REGISTER.MAIN</v>
+      </c>
+      <c r="B112" t="str">
+        <v>Apply and Register</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>SIDENAV.APPLY_REGISTER.REGISTRATION</v>
+      </c>
+      <c r="B113" t="str">
+        <v>Exam Registration</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>SIDENAV.APPLY_REGISTER.REQUIREMENTS</v>
+      </c>
+      <c r="B114" t="str">
+        <v>Registration Requirements</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>SIDENAV.CME</v>
+      </c>
+      <c r="B115" t="str">
+        <v>CME Repository</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>SIDENAV.CONTINUOUS_CERTIFICATION</v>
+      </c>
+      <c r="B116" t="str">
+        <v>Continuous Certification</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>SIDENAV.DASHBOARD</v>
+      </c>
+      <c r="B117" t="str">
+        <v>Dashboard</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>SIDENAV.DOCUMENTS</v>
+      </c>
+      <c r="B118" t="str">
+        <v>Documents</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>SIDENAV.EXAM_HISTORY</v>
+      </c>
+      <c r="B119" t="str">
+        <v>Exam History</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>SIDENAV.EXAM_SCORING.CASE_ROSTER</v>
+      </c>
+      <c r="B120" t="str">
+        <v>Examination Case Rosters</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>SIDENAV.EXAM_SCORING.EXAMINATION</v>
+      </c>
+      <c r="B121" t="str">
+        <v>Deliver CE Exams</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>SIDENAV.EXAM_SCORING.MAIN</v>
+      </c>
+      <c r="B122" t="str">
+        <v>CE Examiner Home</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
         <v>SIDENAV.EXAM_SCORING.SCORES</v>
       </c>
-      <c r="B96" t="str">
+      <c r="B123" t="str">
         <v>Examination Scores</v>
       </c>
     </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>SIDENAV.GME</v>
+      </c>
+      <c r="B124" t="str">
+        <v>GME</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>SIDENAV.MEDICAL_TRAINING</v>
+      </c>
+      <c r="B125" t="str">
+        <v>Medical Training</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>SIDENAV.MYACCOUNT</v>
+      </c>
+      <c r="B126" t="str">
+        <v>My Account</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>SIDENAV.PAYMENT_HISTORY</v>
+      </c>
+      <c r="B127" t="str">
+        <v>Payment History</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>SIDENAV.PROFESSIONAL_STANDING</v>
+      </c>
+      <c r="B128" t="str">
+        <v>Professional Standing</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>SIDENAV.PROFILE</v>
+      </c>
+      <c r="B129" t="str">
+        <v>Personal Profile</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C95"/>
+  <autoFilter ref="A1:D128"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C96"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D129"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>